<commit_message>
Change to CSV file reading for questions data
</commit_message>
<xml_diff>
--- a/data/important_factors_options.xlsx
+++ b/data/important_factors_options.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\伊藤駿\Desktop\適職診断サイト作成\ウェブサイト構築\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_tekishokusindanwebsite\website\myapp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06C5986D-A057-4463-B1A8-53F821625628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1F6FB5-FFE6-4F62-9AEB-AF4523CE13D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{FA5AE2E1-C22F-49E6-81FE-9A91D8E2B383}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11295" xr2:uid="{FA5AE2E1-C22F-49E6-81FE-9A91D8E2B383}"/>
   </bookViews>
   <sheets>
     <sheet name="職種選択で大事にしたいこと質問" sheetId="1" r:id="rId1"/>
@@ -36,128 +36,121 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t>職種選択で大事にしたいこと選択肢</t>
+    <t>職種選択で選択肢</t>
     <rPh sb="0" eb="4">
       <t>ショクシュセンタク</t>
     </rPh>
+    <rPh sb="5" eb="8">
+      <t>センタクシ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>個人の成長と学び</t>
+    <rPh sb="0" eb="2">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>セイチョウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>マナ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>報酬と評価</t>
+    <rPh sb="0" eb="2">
+      <t>ホウシュウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヒョウカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>社会貢献</t>
+    <rPh sb="0" eb="4">
+      <t>シャカイコウケン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>倫理と道徳性</t>
+    <rPh sb="0" eb="2">
+      <t>リンリ</t>
+    </rPh>
+    <rPh sb="3" eb="6">
+      <t>ドウトクセイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>仕事の質と成果</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>シツ</t>
+    </rPh>
     <rPh sb="5" eb="7">
-      <t>ダイジ</t>
-    </rPh>
-    <rPh sb="13" eb="16">
-      <t>センタクシ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>大事にしたいこと1(個人の成長と学び)</t>
-    <rPh sb="0" eb="2">
-      <t>ダイジ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>コジン</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>セイチョウ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>マナ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>大事にしたいこと2(社会貢献)</t>
-    <rPh sb="10" eb="14">
-      <t>シャカイコウケン</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>大事にしたいこと3(仕事の質と成果)</t>
-    <rPh sb="10" eb="12">
-      <t>シゴト</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>シツ</t>
-    </rPh>
-    <rPh sb="15" eb="17">
       <t>セイカ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと4(創造性とイノベーション)</t>
-    <rPh sb="10" eb="13">
+    <t>創造性とイノベーション</t>
+    <rPh sb="0" eb="3">
       <t>ソウゾウセイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと5(協力とチームワーク)</t>
-    <rPh sb="10" eb="12">
+    <t>協力とチームワーク</t>
+    <rPh sb="0" eb="2">
       <t>キョウリョク</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと6(自由と柔軟性)</t>
-    <rPh sb="10" eb="12">
+    <t>自由と柔軟性</t>
+    <rPh sb="0" eb="2">
       <t>ジユウ</t>
     </rPh>
-    <rPh sb="13" eb="16">
+    <rPh sb="3" eb="6">
       <t>ジュウナンセイ</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと7(安定と安全)</t>
-    <rPh sb="10" eb="12">
+    <t>安定と安全</t>
+    <rPh sb="0" eb="2">
       <t>アンテイ</t>
     </rPh>
-    <rPh sb="13" eb="15">
+    <rPh sb="3" eb="5">
       <t>アンゼン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと8(リーダーシップと影響力)</t>
-    <rPh sb="18" eb="21">
+    <t>リーダーシップと影響力</t>
+    <rPh sb="8" eb="11">
       <t>エイキョウリョク</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと9(冒険と挑戦)</t>
-    <rPh sb="10" eb="12">
+    <t>冒険と挑戦</t>
+    <rPh sb="0" eb="2">
       <t>ボウケン</t>
     </rPh>
-    <rPh sb="13" eb="15">
+    <rPh sb="3" eb="5">
       <t>チョウセン</t>
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>大事にしたいこと10(ワークライフバランス)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>大事にしたいこと11(報酬と評価)</t>
-    <rPh sb="11" eb="13">
-      <t>ホウシュウ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>ヒョウカ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>大事にしたいこと12(倫理と道徳性)</t>
-    <rPh sb="11" eb="13">
-      <t>リンリ</t>
-    </rPh>
-    <rPh sb="14" eb="17">
-      <t>ドウトクセイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
+    <t>ワークライフバランス</t>
   </si>
 </sst>
 </file>
@@ -561,7 +554,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84891B7-98DD-4D6B-90DE-10252A3AB42B}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -580,57 +575,57 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>